<commit_message>
Add new methods, add F1-score evaluation
</commit_message>
<xml_diff>
--- a/paper/TableDatasets.xlsx
+++ b/paper/TableDatasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,15 +456,25 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Positive Instances</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Negative Instances</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Features</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Dimensionality</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Balance</t>
         </is>
@@ -493,12 +503,18 @@
         <v>114</v>
       </c>
       <c r="F2" t="n">
+        <v>63</v>
+      </c>
+      <c r="G2" t="n">
+        <v>51</v>
+      </c>
+      <c r="H2" t="n">
         <v>108</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.96</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>55</v>
       </c>
     </row>
@@ -525,12 +541,18 @@
         <v>168</v>
       </c>
       <c r="F3" t="n">
+        <v>111</v>
+      </c>
+      <c r="G3" t="n">
+        <v>57</v>
+      </c>
+      <c r="H3" t="n">
         <v>683</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>4.08</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>66</v>
       </c>
     </row>
@@ -557,12 +579,18 @@
         <v>577</v>
       </c>
       <c r="F4" t="n">
+        <v>301</v>
+      </c>
+      <c r="G4" t="n">
+        <v>276</v>
+      </c>
+      <c r="H4" t="n">
         <v>4060</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>7.04</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>52</v>
       </c>
     </row>
@@ -589,12 +617,18 @@
         <v>58</v>
       </c>
       <c r="F5" t="n">
+        <v>35</v>
+      </c>
+      <c r="G5" t="n">
+        <v>23</v>
+      </c>
+      <c r="H5" t="n">
         <v>2380</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>41.07</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>60</v>
       </c>
     </row>
@@ -621,12 +655,18 @@
         <v>70</v>
       </c>
       <c r="F6" t="n">
+        <v>46</v>
+      </c>
+      <c r="G6" t="n">
+        <v>24</v>
+      </c>
+      <c r="H6" t="n">
         <v>315</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>4.53</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>66</v>
       </c>
     </row>
@@ -653,12 +693,18 @@
         <v>90</v>
       </c>
       <c r="F7" t="n">
+        <v>76</v>
+      </c>
+      <c r="G7" t="n">
+        <v>14</v>
+      </c>
+      <c r="H7" t="n">
         <v>525</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>5.86</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>84</v>
       </c>
     </row>
@@ -685,12 +731,18 @@
         <v>119</v>
       </c>
       <c r="F8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G8" t="n">
+        <v>88</v>
+      </c>
+      <c r="H8" t="n">
         <v>851</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>7.17</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>26</v>
       </c>
     </row>
@@ -717,12 +769,18 @@
         <v>261</v>
       </c>
       <c r="F9" t="n">
+        <v>94</v>
+      </c>
+      <c r="G9" t="n">
+        <v>167</v>
+      </c>
+      <c r="H9" t="n">
         <v>225</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.87</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>36</v>
       </c>
     </row>
@@ -749,12 +807,18 @@
         <v>279</v>
       </c>
       <c r="F10" t="n">
+        <v>136</v>
+      </c>
+      <c r="G10" t="n">
+        <v>143</v>
+      </c>
+      <c r="H10" t="n">
         <v>851</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>3.06</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>49</v>
       </c>
     </row>
@@ -781,12 +845,18 @@
         <v>54</v>
       </c>
       <c r="F11" t="n">
+        <v>33</v>
+      </c>
+      <c r="G11" t="n">
+        <v>21</v>
+      </c>
+      <c r="H11" t="n">
         <v>192</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>3.59</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>61</v>
       </c>
     </row>
@@ -813,12 +883,18 @@
         <v>88</v>
       </c>
       <c r="F12" t="n">
+        <v>41</v>
+      </c>
+      <c r="G12" t="n">
+        <v>47</v>
+      </c>
+      <c r="H12" t="n">
         <v>580</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>6.61</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>47</v>
       </c>
     </row>
@@ -845,12 +921,18 @@
         <v>51</v>
       </c>
       <c r="F13" t="n">
+        <v>38</v>
+      </c>
+      <c r="G13" t="n">
+        <v>13</v>
+      </c>
+      <c r="H13" t="n">
         <v>851</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>16.73</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>75</v>
       </c>
     </row>
@@ -877,12 +959,18 @@
         <v>84</v>
       </c>
       <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>72</v>
+      </c>
+      <c r="H14" t="n">
         <v>420</v>
       </c>
-      <c r="G14" t="n">
+      <c r="I14" t="n">
         <v>5.02</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>14</v>
       </c>
     </row>
@@ -909,12 +997,18 @@
         <v>93</v>
       </c>
       <c r="F15" t="n">
+        <v>25</v>
+      </c>
+      <c r="G15" t="n">
+        <v>68</v>
+      </c>
+      <c r="H15" t="n">
         <v>105</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>1.15</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>27</v>
       </c>
     </row>
@@ -941,12 +1035,18 @@
         <v>91</v>
       </c>
       <c r="F16" t="n">
+        <v>61</v>
+      </c>
+      <c r="G16" t="n">
+        <v>30</v>
+      </c>
+      <c r="H16" t="n">
         <v>210</v>
       </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
         <v>2.33</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>67</v>
       </c>
     </row>
@@ -973,12 +1073,18 @@
         <v>137</v>
       </c>
       <c r="F17" t="n">
+        <v>61</v>
+      </c>
+      <c r="G17" t="n">
+        <v>76</v>
+      </c>
+      <c r="H17" t="n">
         <v>105</v>
       </c>
-      <c r="G17" t="n">
+      <c r="I17" t="n">
         <v>0.78</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>45</v>
       </c>
     </row>
@@ -1005,12 +1111,18 @@
         <v>293</v>
       </c>
       <c r="F18" t="n">
+        <v>159</v>
+      </c>
+      <c r="G18" t="n">
+        <v>134</v>
+      </c>
+      <c r="H18" t="n">
         <v>984</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>3.37</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>54</v>
       </c>
     </row>
@@ -1037,12 +1149,18 @@
         <v>207</v>
       </c>
       <c r="F19" t="n">
+        <v>60</v>
+      </c>
+      <c r="G19" t="n">
+        <v>147</v>
+      </c>
+      <c r="H19" t="n">
         <v>984</v>
       </c>
-      <c r="G19" t="n">
+      <c r="I19" t="n">
         <v>4.76</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1069,12 +1187,18 @@
         <v>183</v>
       </c>
       <c r="F20" t="n">
+        <v>133</v>
+      </c>
+      <c r="G20" t="n">
+        <v>50</v>
+      </c>
+      <c r="H20" t="n">
         <v>984</v>
       </c>
-      <c r="G20" t="n">
+      <c r="I20" t="n">
         <v>5.39</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
         <v>73</v>
       </c>
     </row>
@@ -1101,12 +1225,18 @@
         <v>212</v>
       </c>
       <c r="F21" t="n">
+        <v>97</v>
+      </c>
+      <c r="G21" t="n">
+        <v>115</v>
+      </c>
+      <c r="H21" t="n">
         <v>855</v>
       </c>
-      <c r="G21" t="n">
+      <c r="I21" t="n">
         <v>4.04</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
         <v>46</v>
       </c>
     </row>
@@ -1133,12 +1263,18 @@
         <v>520</v>
       </c>
       <c r="F22" t="n">
+        <v>282</v>
+      </c>
+      <c r="G22" t="n">
+        <v>238</v>
+      </c>
+      <c r="H22" t="n">
         <v>1998</v>
       </c>
-      <c r="G22" t="n">
+      <c r="I22" t="n">
         <v>3.85</v>
       </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
         <v>54</v>
       </c>
     </row>
@@ -1165,12 +1301,18 @@
         <v>161</v>
       </c>
       <c r="F23" t="n">
+        <v>92</v>
+      </c>
+      <c r="G23" t="n">
+        <v>69</v>
+      </c>
+      <c r="H23" t="n">
         <v>370</v>
       </c>
-      <c r="G23" t="n">
+      <c r="I23" t="n">
         <v>2.31</v>
       </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
         <v>57</v>
       </c>
     </row>
@@ -1197,12 +1339,18 @@
         <v>273</v>
       </c>
       <c r="F24" t="n">
+        <v>119</v>
+      </c>
+      <c r="G24" t="n">
+        <v>154</v>
+      </c>
+      <c r="H24" t="n">
         <v>1322</v>
       </c>
-      <c r="G24" t="n">
+      <c r="I24" t="n">
         <v>4.85</v>
       </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
         <v>44</v>
       </c>
     </row>
@@ -1229,12 +1377,18 @@
         <v>159</v>
       </c>
       <c r="F25" t="n">
+        <v>102</v>
+      </c>
+      <c r="G25" t="n">
+        <v>57</v>
+      </c>
+      <c r="H25" t="n">
         <v>2030</v>
       </c>
-      <c r="G25" t="n">
+      <c r="I25" t="n">
         <v>12.78</v>
       </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1261,12 +1415,18 @@
         <v>173</v>
       </c>
       <c r="F26" t="n">
+        <v>115</v>
+      </c>
+      <c r="G26" t="n">
+        <v>58</v>
+      </c>
+      <c r="H26" t="n">
         <v>105</v>
       </c>
-      <c r="G26" t="n">
+      <c r="I26" t="n">
         <v>0.62</v>
       </c>
-      <c r="H26" t="n">
+      <c r="J26" t="n">
         <v>66</v>
       </c>
     </row>
@@ -1293,12 +1453,18 @@
         <v>51</v>
       </c>
       <c r="F27" t="n">
+        <v>32</v>
+      </c>
+      <c r="G27" t="n">
+        <v>19</v>
+      </c>
+      <c r="H27" t="n">
         <v>396</v>
       </c>
-      <c r="G27" t="n">
+      <c r="I27" t="n">
         <v>7.8</v>
       </c>
-      <c r="H27" t="n">
+      <c r="J27" t="n">
         <v>63</v>
       </c>
     </row>
@@ -1325,12 +1491,18 @@
         <v>75</v>
       </c>
       <c r="F28" t="n">
+        <v>55</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20</v>
+      </c>
+      <c r="H28" t="n">
         <v>657</v>
       </c>
-      <c r="G28" t="n">
+      <c r="I28" t="n">
         <v>8.789999999999999</v>
       </c>
-      <c r="H28" t="n">
+      <c r="J28" t="n">
         <v>73</v>
       </c>
     </row>
@@ -1357,12 +1529,18 @@
         <v>88</v>
       </c>
       <c r="F29" t="n">
+        <v>38</v>
+      </c>
+      <c r="G29" t="n">
+        <v>50</v>
+      </c>
+      <c r="H29" t="n">
         <v>2030</v>
       </c>
-      <c r="G29" t="n">
+      <c r="I29" t="n">
         <v>23.09</v>
       </c>
-      <c r="H29" t="n">
+      <c r="J29" t="n">
         <v>43</v>
       </c>
     </row>
@@ -1389,12 +1567,18 @@
         <v>144</v>
       </c>
       <c r="F30" t="n">
+        <v>23</v>
+      </c>
+      <c r="G30" t="n">
+        <v>121</v>
+      </c>
+      <c r="H30" t="n">
         <v>105</v>
       </c>
-      <c r="G30" t="n">
+      <c r="I30" t="n">
         <v>0.74</v>
       </c>
-      <c r="H30" t="n">
+      <c r="J30" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1421,12 +1605,18 @@
         <v>67</v>
       </c>
       <c r="F31" t="n">
+        <v>32</v>
+      </c>
+      <c r="G31" t="n">
+        <v>35</v>
+      </c>
+      <c r="H31" t="n">
         <v>1130</v>
       </c>
-      <c r="G31" t="n">
+      <c r="I31" t="n">
         <v>16.9</v>
       </c>
-      <c r="H31" t="n">
+      <c r="J31" t="n">
         <v>48</v>
       </c>
     </row>
@@ -1453,12 +1643,18 @@
         <v>969</v>
       </c>
       <c r="F32" t="n">
+        <v>637</v>
+      </c>
+      <c r="G32" t="n">
+        <v>332</v>
+      </c>
+      <c r="H32" t="n">
         <v>3045</v>
       </c>
-      <c r="G32" t="n">
+      <c r="I32" t="n">
         <v>3.14</v>
       </c>
-      <c r="H32" t="n">
+      <c r="J32" t="n">
         <v>66</v>
       </c>
     </row>
@@ -1485,12 +1681,18 @@
         <v>128</v>
       </c>
       <c r="F33" t="n">
+        <v>47</v>
+      </c>
+      <c r="G33" t="n">
+        <v>81</v>
+      </c>
+      <c r="H33" t="n">
         <v>851</v>
       </c>
-      <c r="G33" t="n">
+      <c r="I33" t="n">
         <v>6.66</v>
       </c>
-      <c r="H33" t="n">
+      <c r="J33" t="n">
         <v>37</v>
       </c>
     </row>
@@ -1517,12 +1719,18 @@
         <v>773</v>
       </c>
       <c r="F34" t="n">
+        <v>596</v>
+      </c>
+      <c r="G34" t="n">
+        <v>177</v>
+      </c>
+      <c r="H34" t="n">
         <v>1015</v>
       </c>
-      <c r="G34" t="n">
+      <c r="I34" t="n">
         <v>1.32</v>
       </c>
-      <c r="H34" t="n">
+      <c r="J34" t="n">
         <v>77</v>
       </c>
     </row>
@@ -1549,12 +1757,18 @@
         <v>59</v>
       </c>
       <c r="F35" t="n">
+        <v>44</v>
+      </c>
+      <c r="G35" t="n">
+        <v>15</v>
+      </c>
+      <c r="H35" t="n">
         <v>210</v>
       </c>
-      <c r="G35" t="n">
+      <c r="I35" t="n">
         <v>3.59</v>
       </c>
-      <c r="H35" t="n">
+      <c r="J35" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1581,12 +1795,18 @@
         <v>91</v>
       </c>
       <c r="F36" t="n">
+        <v>50</v>
+      </c>
+      <c r="G36" t="n">
+        <v>41</v>
+      </c>
+      <c r="H36" t="n">
         <v>242</v>
       </c>
-      <c r="G36" t="n">
+      <c r="I36" t="n">
         <v>2.68</v>
       </c>
-      <c r="H36" t="n">
+      <c r="J36" t="n">
         <v>55</v>
       </c>
     </row>
@@ -1613,12 +1833,18 @@
         <v>138</v>
       </c>
       <c r="F37" t="n">
+        <v>68</v>
+      </c>
+      <c r="G37" t="n">
+        <v>70</v>
+      </c>
+      <c r="H37" t="n">
         <v>587</v>
       </c>
-      <c r="G37" t="n">
+      <c r="I37" t="n">
         <v>4.27</v>
       </c>
-      <c r="H37" t="n">
+      <c r="J37" t="n">
         <v>49</v>
       </c>
     </row>
@@ -1645,12 +1871,18 @@
         <v>260</v>
       </c>
       <c r="F38" t="n">
+        <v>127</v>
+      </c>
+      <c r="G38" t="n">
+        <v>133</v>
+      </c>
+      <c r="H38" t="n">
         <v>264</v>
       </c>
-      <c r="G38" t="n">
+      <c r="I38" t="n">
         <v>1.02</v>
       </c>
-      <c r="H38" t="n">
+      <c r="J38" t="n">
         <v>49</v>
       </c>
     </row>
@@ -1677,12 +1909,18 @@
         <v>418</v>
       </c>
       <c r="F39" t="n">
+        <v>373</v>
+      </c>
+      <c r="G39" t="n">
+        <v>45</v>
+      </c>
+      <c r="H39" t="n">
         <v>7105</v>
       </c>
-      <c r="G39" t="n">
+      <c r="I39" t="n">
         <v>17</v>
       </c>
-      <c r="H39" t="n">
+      <c r="J39" t="n">
         <v>89</v>
       </c>
     </row>
@@ -1709,12 +1947,18 @@
         <v>187</v>
       </c>
       <c r="F40" t="n">
+        <v>79</v>
+      </c>
+      <c r="G40" t="n">
+        <v>108</v>
+      </c>
+      <c r="H40" t="n">
         <v>11165</v>
       </c>
-      <c r="G40" t="n">
+      <c r="I40" t="n">
         <v>59.72</v>
       </c>
-      <c r="H40" t="n">
+      <c r="J40" t="n">
         <v>42</v>
       </c>
     </row>
@@ -1741,12 +1985,18 @@
         <v>150</v>
       </c>
       <c r="F41" t="n">
+        <v>47</v>
+      </c>
+      <c r="G41" t="n">
+        <v>103</v>
+      </c>
+      <c r="H41" t="n">
         <v>200</v>
       </c>
-      <c r="G41" t="n">
+      <c r="I41" t="n">
         <v>1.35</v>
       </c>
-      <c r="H41" t="n">
+      <c r="J41" t="n">
         <v>31</v>
       </c>
     </row>
@@ -1773,12 +2023,18 @@
         <v>77</v>
       </c>
       <c r="F42" t="n">
+        <v>37</v>
+      </c>
+      <c r="G42" t="n">
+        <v>40</v>
+      </c>
+      <c r="H42" t="n">
         <v>1015</v>
       </c>
-      <c r="G42" t="n">
+      <c r="I42" t="n">
         <v>13.21</v>
       </c>
-      <c r="H42" t="n">
+      <c r="J42" t="n">
         <v>48</v>
       </c>
     </row>
@@ -1805,12 +2061,18 @@
         <v>203</v>
       </c>
       <c r="F43" t="n">
+        <v>72</v>
+      </c>
+      <c r="G43" t="n">
+        <v>131</v>
+      </c>
+      <c r="H43" t="n">
         <v>1015</v>
       </c>
-      <c r="G43" t="n">
+      <c r="I43" t="n">
         <v>5.01</v>
       </c>
-      <c r="H43" t="n">
+      <c r="J43" t="n">
         <v>35</v>
       </c>
     </row>
@@ -1837,12 +2099,18 @@
         <v>245</v>
       </c>
       <c r="F44" t="n">
+        <v>124</v>
+      </c>
+      <c r="G44" t="n">
+        <v>121</v>
+      </c>
+      <c r="H44" t="n">
         <v>1015</v>
       </c>
-      <c r="G44" t="n">
+      <c r="I44" t="n">
         <v>4.15</v>
       </c>
-      <c r="H44" t="n">
+      <c r="J44" t="n">
         <v>51</v>
       </c>
     </row>
@@ -1869,12 +2137,18 @@
         <v>114</v>
       </c>
       <c r="F45" t="n">
+        <v>57</v>
+      </c>
+      <c r="G45" t="n">
+        <v>57</v>
+      </c>
+      <c r="H45" t="n">
         <v>1015</v>
       </c>
-      <c r="G45" t="n">
+      <c r="I45" t="n">
         <v>8.92</v>
       </c>
-      <c r="H45" t="n">
+      <c r="J45" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1901,12 +2175,18 @@
         <v>186</v>
       </c>
       <c r="F46" t="n">
+        <v>94</v>
+      </c>
+      <c r="G46" t="n">
+        <v>92</v>
+      </c>
+      <c r="H46" t="n">
         <v>1015</v>
       </c>
-      <c r="G46" t="n">
+      <c r="I46" t="n">
         <v>5.47</v>
       </c>
-      <c r="H46" t="n">
+      <c r="J46" t="n">
         <v>51</v>
       </c>
     </row>
@@ -1933,12 +2213,18 @@
         <v>95</v>
       </c>
       <c r="F47" t="n">
+        <v>47</v>
+      </c>
+      <c r="G47" t="n">
+        <v>48</v>
+      </c>
+      <c r="H47" t="n">
         <v>1015</v>
       </c>
-      <c r="G47" t="n">
+      <c r="I47" t="n">
         <v>10.71</v>
       </c>
-      <c r="H47" t="n">
+      <c r="J47" t="n">
         <v>49</v>
       </c>
     </row>
@@ -1965,12 +2251,18 @@
         <v>67</v>
       </c>
       <c r="F48" t="n">
+        <v>27</v>
+      </c>
+      <c r="G48" t="n">
+        <v>40</v>
+      </c>
+      <c r="H48" t="n">
         <v>280</v>
       </c>
-      <c r="G48" t="n">
+      <c r="I48" t="n">
         <v>4.21</v>
       </c>
-      <c r="H48" t="n">
+      <c r="J48" t="n">
         <v>40</v>
       </c>
     </row>
@@ -1997,12 +2289,18 @@
         <v>203</v>
       </c>
       <c r="F49" t="n">
+        <v>104</v>
+      </c>
+      <c r="G49" t="n">
+        <v>99</v>
+      </c>
+      <c r="H49" t="n">
         <v>1781</v>
       </c>
-      <c r="G49" t="n">
+      <c r="I49" t="n">
         <v>8.779999999999999</v>
       </c>
-      <c r="H49" t="n">
+      <c r="J49" t="n">
         <v>51</v>
       </c>
     </row>
@@ -2029,12 +2327,18 @@
         <v>255</v>
       </c>
       <c r="F50" t="n">
+        <v>145</v>
+      </c>
+      <c r="G50" t="n">
+        <v>110</v>
+      </c>
+      <c r="H50" t="n">
         <v>3850</v>
       </c>
-      <c r="G50" t="n">
+      <c r="I50" t="n">
         <v>15.11</v>
       </c>
-      <c r="H50" t="n">
+      <c r="J50" t="n">
         <v>57</v>
       </c>
     </row>
@@ -2061,12 +2365,18 @@
         <v>192</v>
       </c>
       <c r="F51" t="n">
+        <v>126</v>
+      </c>
+      <c r="G51" t="n">
+        <v>66</v>
+      </c>
+      <c r="H51" t="n">
         <v>833</v>
       </c>
-      <c r="G51" t="n">
+      <c r="I51" t="n">
         <v>4.35</v>
       </c>
-      <c r="H51" t="n">
+      <c r="J51" t="n">
         <v>66</v>
       </c>
     </row>

</xml_diff>